<commit_message>
Changed VS routing, updated BOM
</commit_message>
<xml_diff>
--- a/power_monitor/Power_Monitor_BOM.xlsx
+++ b/power_monitor/Power_Monitor_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moira\Desktop\Power Monitor\au_hardware\power_monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BE7C56-86E7-4890-A908-7FD24A1AFC2E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C82FBA9-1353-4027-9A64-2D9B039BE74A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{50A2B695-FFBF-4145-A700-70092A451CFF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Shematic Reference Number</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Power Monitor Part List</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>CONN HEADER 2 POS 2.54</t>
   </si>
 </sst>
 </file>
@@ -360,6 +366,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,15 +384,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -694,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483AE8BC-1B46-4E25-B488-E427E5A342C8}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -712,15 +718,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -746,25 +752,25 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="13">
         <v>5.39</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="13">
         <v>1</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="13">
         <v>0</v>
       </c>
       <c r="H3" t="s">
@@ -781,7 +787,7 @@
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="1">
@@ -808,59 +814,83 @@
       <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="10">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <v>1</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="9">
         <f>F5*E5</f>
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="15">
-        <v>61300411121</v>
-      </c>
-      <c r="D6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="12">
+        <v>61300211121</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="F6" s="4">
+      <c r="E6" s="10">
+        <v>0.13</v>
+      </c>
+      <c r="F6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="14">
-        <f>F6*E6</f>
-        <v>0.25</v>
+      <c r="G6" s="9">
+        <v>0.13</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F7" s="5" t="s">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="12">
+        <v>61300411121</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11">
+        <f>F7*E7</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="6">
-        <f>SUM(G3:G6)</f>
-        <v>2.85</v>
+      <c r="G8" s="6">
+        <f>SUM(G3:G7)</f>
+        <v>2.98</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{49AFABEE-7F8E-400F-ADCE-3CF0FE953021}"/>
-    <hyperlink ref="D6" r:id="rId2" xr:uid="{F013344C-09FC-47C4-AF1F-C39B6B7370F1}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{F013344C-09FC-47C4-AF1F-C39B6B7370F1}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{3F7F5AD6-DCE7-452B-A968-46004CD054BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>